<commit_message>
new coin and fish coords
</commit_message>
<xml_diff>
--- a/Background_coord_fish.xlsx
+++ b/Background_coord_fish.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0717837\Documents\GitHub\Rapid-P2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Rapid-P2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$36</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,33 +482,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>313</v>
+        <v>106</v>
       </c>
       <c r="C3">
-        <v>1306</v>
+        <v>1526</v>
       </c>
       <c r="D3">
         <v>4</v>
       </c>
       <c r="E3">
         <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>466</v>
-      </c>
-      <c r="C4">
-        <v>2304</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -513,7 +499,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>878</v>
+        <v>828</v>
       </c>
       <c r="C5">
         <v>2566</v>
@@ -542,23 +528,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>600</v>
-      </c>
-      <c r="C7">
-        <v>3121</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
@@ -593,46 +562,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>1256</v>
-      </c>
-      <c r="C10">
-        <v>3338</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>494</v>
-      </c>
-      <c r="C11">
-        <v>4010</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1362</v>
+        <v>1332</v>
       </c>
       <c r="C12">
         <v>2920</v>
@@ -785,32 +720,15 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>1092</v>
+        <v>1112</v>
       </c>
       <c r="C21">
-        <v>6644</v>
+        <v>6664</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>588</v>
-      </c>
-      <c r="C22">
-        <v>7169</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22">
         <v>0</v>
       </c>
     </row>
@@ -819,7 +737,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <v>7268</v>
@@ -836,10 +754,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>1041</v>
+        <v>1141</v>
       </c>
       <c r="C24">
-        <v>7378</v>
+        <v>7428</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -870,10 +788,10 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>1081</v>
+        <v>1031</v>
       </c>
       <c r="C26">
-        <v>7976</v>
+        <v>7946</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -904,7 +822,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>188</v>
+        <v>128</v>
       </c>
       <c r="C28">
         <v>8973</v>
@@ -921,10 +839,10 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>297</v>
+        <v>10</v>
       </c>
       <c r="C29">
-        <v>8654</v>
+        <v>8754</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -984,27 +902,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:E36"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>